<commit_message>
#173 header css 만
</commit_message>
<xml_diff>
--- a/0. document/2. 보고서/6차 보고서_마일스톤 상세.xlsx
+++ b/0. document/2. 보고서/6차 보고서_마일스톤 상세.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E7F9AF2-BEA0-4F60-A6F2-F673C8CB1DF0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF0B944-E525-4978-B92D-3587EDA27EED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="1095" windowWidth="19425" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="1695" windowWidth="19425" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -617,7 +617,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -630,6 +629,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - 강조색2" xfId="1" builtinId="34"/>
@@ -1357,7 +1357,7 @@
   <dimension ref="A1:O68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1490,10 +1490,10 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="28"/>
+      <c r="B8" s="27"/>
       <c r="D8" s="5" t="s">
         <v>31</v>
       </c>
@@ -1511,10 +1511,10 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="28"/>
+      <c r="B9" s="27"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5" t="s">
         <v>31</v>
@@ -1548,10 +1548,10 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="28"/>
+      <c r="B10" s="27"/>
       <c r="M10" s="5" t="s">
         <v>31</v>
       </c>
@@ -1563,10 +1563,10 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="26"/>
+      <c r="B11" s="25"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
@@ -1590,10 +1590,10 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="28"/>
+      <c r="B12" s="27"/>
       <c r="D12" t="s">
         <v>42</v>
       </c>
@@ -1612,8 +1612,8 @@
       <c r="I12" t="s">
         <v>64</v>
       </c>
-      <c r="J12" t="s">
-        <v>70</v>
+      <c r="J12" s="17" t="s">
+        <v>84</v>
       </c>
       <c r="K12" t="s">
         <v>73</v>
@@ -1638,8 +1638,8 @@
         <v>45</v>
       </c>
       <c r="I13" s="23"/>
-      <c r="J13" t="s">
-        <v>71</v>
+      <c r="J13" s="17" t="s">
+        <v>85</v>
       </c>
       <c r="K13" t="s">
         <v>74</v>
@@ -1658,11 +1658,14 @@
         <v>40</v>
       </c>
       <c r="I14" s="23"/>
-      <c r="J14" t="s">
-        <v>72</v>
+      <c r="J14" s="17" t="s">
+        <v>86</v>
       </c>
       <c r="K14" t="s">
         <v>75</v>
+      </c>
+      <c r="L14" t="s">
+        <v>70</v>
       </c>
       <c r="M14" s="21" t="s">
         <v>89</v>
@@ -1678,8 +1681,8 @@
       <c r="K15" t="s">
         <v>76</v>
       </c>
-      <c r="L15" s="17" t="s">
-        <v>84</v>
+      <c r="L15" t="s">
+        <v>71</v>
       </c>
       <c r="M15" s="22"/>
     </row>
@@ -1693,22 +1696,19 @@
       <c r="K16" t="s">
         <v>77</v>
       </c>
-      <c r="L16" s="17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="11"/>
       <c r="B17" s="12"/>
       <c r="I17" s="23"/>
       <c r="K17" t="s">
         <v>78</v>
       </c>
-      <c r="L17" s="17" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
       <c r="B18" s="12"/>
       <c r="I18" s="23"/>
@@ -1716,7 +1716,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="11"/>
       <c r="B19" s="12"/>
       <c r="I19" s="23"/>
@@ -1724,22 +1724,22 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="11"/>
       <c r="B20" s="12"/>
       <c r="I20" s="23"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="11"/>
       <c r="B21" s="12"/>
       <c r="I21" s="23"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="11"/>
       <c r="B22" s="12"/>
       <c r="I22" s="23"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="11"/>
       <c r="B23" s="12"/>
       <c r="F23" t="s">
@@ -1749,28 +1749,28 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="11"/>
       <c r="B24" s="12"/>
       <c r="I24" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
       <c r="B25" s="12"/>
       <c r="I25" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="11"/>
       <c r="B26" s="12"/>
       <c r="I26" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="11"/>
       <c r="B27" s="12"/>
       <c r="H27" t="s">
@@ -1780,7 +1780,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="11"/>
       <c r="B28" s="12"/>
       <c r="H28" t="s">
@@ -1790,7 +1790,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="11"/>
       <c r="B29" s="12"/>
       <c r="H29" t="s">
@@ -1800,15 +1800,15 @@
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="11"/>
       <c r="B30" s="12"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="11"/>
       <c r="B31" s="12"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="11"/>
       <c r="B32" s="12"/>
     </row>
@@ -1853,27 +1853,27 @@
       <c r="B39" s="10"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="24"/>
-      <c r="B42" s="24"/>
+      <c r="A42" s="28"/>
+      <c r="B42" s="28"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="24"/>
-      <c r="B43" s="24"/>
+      <c r="A43" s="28"/>
+      <c r="B43" s="28"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="24"/>
-      <c r="B44" s="24"/>
+      <c r="A44" s="28"/>
+      <c r="B44" s="28"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="24"/>
-      <c r="B45" s="24"/>
+      <c r="A45" s="28"/>
+      <c r="B45" s="28"/>
       <c r="G45" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="24"/>
-      <c r="B46" s="24"/>
+      <c r="A46" s="28"/>
+      <c r="B46" s="28"/>
       <c r="F46" t="s">
         <v>48</v>
       </c>
@@ -1882,24 +1882,24 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="24"/>
-      <c r="B50" s="24"/>
+      <c r="A50" s="28"/>
+      <c r="B50" s="28"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="24"/>
-      <c r="B51" s="24"/>
+      <c r="A51" s="28"/>
+      <c r="B51" s="28"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="24"/>
-      <c r="B52" s="24"/>
+      <c r="A52" s="28"/>
+      <c r="B52" s="28"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="24"/>
-      <c r="B53" s="24"/>
+      <c r="A53" s="28"/>
+      <c r="B53" s="28"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="24"/>
-      <c r="B54" s="24"/>
+      <c r="A54" s="28"/>
+      <c r="B54" s="28"/>
       <c r="G54" t="s">
         <v>56</v>
       </c>
@@ -1915,6 +1915,12 @@
     <row r="68" spans="4:4" ht="17.25" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A51:B51"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A46:B46"/>
@@ -1924,12 +1930,6 @@
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A51:B51"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#182 지도 아이콘 클릭시 rightmenu groupinfo 페이지완료 (#183)
</commit_message>
<xml_diff>
--- a/0. document/2. 보고서/6차 보고서_마일스톤 상세.xlsx
+++ b/0. document/2. 보고서/6차 보고서_마일스톤 상세.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819844E6-EE44-4956-B89B-718C5EB0CABF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E89ACF2-4313-452D-AE3F-DB3D1349AC07}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="490" windowWidth="19420" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,7 +574,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -618,6 +618,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -630,7 +631,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - 강조색2" xfId="1" builtinId="34"/>
@@ -1358,7 +1359,7 @@
   <dimension ref="A1:O68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1491,10 +1492,10 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="28"/>
+      <c r="B8" s="29"/>
       <c r="D8" s="5" t="s">
         <v>31</v>
       </c>
@@ -1512,10 +1513,10 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="28"/>
+      <c r="B9" s="29"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5" t="s">
         <v>31</v>
@@ -1549,10 +1550,10 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="28"/>
+      <c r="B10" s="29"/>
       <c r="M10" s="5" t="s">
         <v>31</v>
       </c>
@@ -1564,10 +1565,10 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="26"/>
+      <c r="B11" s="27"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
@@ -1591,10 +1592,10 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="28"/>
+      <c r="B12" s="29"/>
       <c r="D12" t="s">
         <v>42</v>
       </c>
@@ -1642,7 +1643,7 @@
       <c r="J13" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="K13" s="29" t="s">
+      <c r="K13" s="25" t="s">
         <v>74</v>
       </c>
       <c r="L13" s="17" t="s">
@@ -1702,7 +1703,7 @@
       <c r="A17" s="11"/>
       <c r="B17" s="12"/>
       <c r="I17" s="23"/>
-      <c r="K17" s="29" t="s">
+      <c r="K17" s="25" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1726,7 +1727,7 @@
       <c r="A20" s="11"/>
       <c r="B20" s="12"/>
       <c r="I20" s="23"/>
-      <c r="K20" s="17" t="s">
+      <c r="K20" s="25" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1734,6 +1735,7 @@
       <c r="A21" s="11"/>
       <c r="B21" s="12"/>
       <c r="I21" s="23"/>
+      <c r="K21" s="24"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="11"/>
@@ -1854,27 +1856,27 @@
       <c r="B39" s="10"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A42" s="24"/>
-      <c r="B42" s="24"/>
+      <c r="A42" s="30"/>
+      <c r="B42" s="30"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A43" s="24"/>
-      <c r="B43" s="24"/>
+      <c r="A43" s="30"/>
+      <c r="B43" s="30"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A44" s="24"/>
-      <c r="B44" s="24"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="30"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A45" s="24"/>
-      <c r="B45" s="24"/>
+      <c r="A45" s="30"/>
+      <c r="B45" s="30"/>
       <c r="G45" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A46" s="24"/>
-      <c r="B46" s="24"/>
+      <c r="A46" s="30"/>
+      <c r="B46" s="30"/>
       <c r="F46" t="s">
         <v>48</v>
       </c>
@@ -1883,24 +1885,24 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A50" s="24"/>
-      <c r="B50" s="24"/>
+      <c r="A50" s="30"/>
+      <c r="B50" s="30"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A51" s="24"/>
-      <c r="B51" s="24"/>
+      <c r="A51" s="30"/>
+      <c r="B51" s="30"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A52" s="24"/>
-      <c r="B52" s="24"/>
+      <c r="A52" s="30"/>
+      <c r="B52" s="30"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A53" s="24"/>
-      <c r="B53" s="24"/>
+      <c r="A53" s="30"/>
+      <c r="B53" s="30"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A54" s="24"/>
-      <c r="B54" s="24"/>
+      <c r="A54" s="30"/>
+      <c r="B54" s="30"/>
       <c r="G54" t="s">
         <v>56</v>
       </c>
@@ -1916,6 +1918,12 @@
     <row r="68" spans="4:4" ht="17.5" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A51:B51"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A46:B46"/>
@@ -1925,12 +1933,6 @@
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A51:B51"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>